<commit_message>
Add CN A Shares price history; Add Nasdaq price info of 10y.
</commit_message>
<xml_diff>
--- a/stock_data_description.xlsx
+++ b/stock_data_description.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>数据集</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,10 +142,6 @@
   </si>
   <si>
     <t>新浪财经(http://vip.stock.finance.sina.com.cn/usstock/ustotal.php)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nasdaq主要股票十年的价格数据。每只股票对应一个文件，文件名为股票名称。文件每行格式为：[date + "\t" + open + "\t" + high + "\t" + low + "\t" + close + "\t" + volume]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -250,6 +246,60 @@
   </si>
   <si>
     <t>https://github.com/zeyazhang/sewm_stock_data/blob/master/SeekingAlphaUsStockNews.rar</t>
+  </si>
+  <si>
+    <t>(9)A股3000只股票历史价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19910101-20170620</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>161M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;100M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接: https://pan.baidu.com/s/1nvPZK6X 密码: i5ae</t>
+  </si>
+  <si>
+    <t>复权后的价格数据。格式为[date, open, high, close, low, ?, volume]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由白天煜同学提供。使用Python的Tushare包获取。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10)Nasdaq6000只股票10年数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20070618-20170616</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>125M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接: https://pan.baidu.com/s/1nvhu3CP 密码: sfwx</t>
+  </si>
+  <si>
+    <t>Nasdaq主要股票十年的价格数据。每只股票对应一个文件，文件名为股票名称。文件每行格式为：[date + "\t" + open + "\t" + high + "\t" + low + "\t" + close + "\t" + volume]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nasdaq市场股票十年的价格数据。每只股票对应一个文件。文件每行格式为：[date + "\t" + open + "\t" + high + "\t" + low + "\t" + close + "\t" + volume]。【注意】部分股票价格不全（那些只有65天数据的），可设置爬虫程序，让程序在请求数据后等待更长时间，以获得完全的数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纳斯达克官网http://www.nasdaq.com/symbol/[symbol]/historical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -614,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -642,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -656,7 +706,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -664,19 +714,22 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -685,21 +738,21 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -708,21 +761,21 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -731,7 +784,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -745,7 +798,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -754,7 +807,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -768,7 +821,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -777,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -791,7 +844,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -800,7 +853,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -811,7 +864,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -820,16 +873,62 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>